<commit_message>
1.open include head dedup switch;2.fix val_declare defination none;3.add cu files to scanner;4.extend enum api compare result
</commit_message>
<xml_diff>
--- a/ait/components/analyze/app/config/ACL_API_MAP.xlsx
+++ b/ait/components/analyze/app/config/ACL_API_MAP.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lisa\AppData\Local\Temp\Mxt231\RemoteFiles\855638_4_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lisa\AppData\Local\Temp\Mxt231\RemoteFiles\855638_6_22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D05510-EC91-458C-9E7C-90EB1BB36D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22F1F01-F691-440D-BE64-EE0F7C0FEB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ACL-CUDARuntime-APIMap" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="313">
   <si>
     <t>迁移预估人力（人/天）</t>
   </si>
@@ -687,10 +687,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>入参映射关系</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>cudaGetLastError</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1218,10 +1214,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>cudaMemoryType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>enum cudaMemoryType {
 cudaMemoryTypeUnregistered = 0,
 cudaMemoryTypeHost = 1,
@@ -1243,43 +1235,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>函数功能</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>昇腾</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>API</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>说明</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>备注</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>API</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>昇腾</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>CUDA Runtime</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>CUDA</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">	cudaRuntimeGetVersion</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -1294,6 +1250,164 @@
     <t>majorVersion：int32_t*
 minorVersion：int32_t*
 patchVersion：int32_t*</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>昇腾API</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>昇腾API参数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>详情</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>cudaRuntimeGetVersion</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA Runtime API参数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NV_API</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>cudaError.cudaSuccess</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>执行成功</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACL_SUCCESS</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>错误码</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>上下文</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>流</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>内存类型</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>aclMemType.ACL_MEMTYPE_DEVICE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>udaMemoryType.cudaMemoryTypeDevice</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>aclMemType.ACL_MEMTYPE_HOST</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>udaMemoryType.cudaMemoryTypeHost</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>device内存</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>host内存</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">aclrtMemcpyKind </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>内存复制的类型</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>cudaMemcpyKind</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum cudaMemcpyKind {
+cudaMemcpyHostToHost = 0,
+cudaMemcpyHostToDevice = 1,
+cudaMemcpyDeviceToHost = 2,
+cudaMemcpyDeviceToDevice = 3,
+cudaMemcpyDefault = 4}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>typedef enum aclrtMemcpyKind {
+ACL_MEMCPY_HOST_TO_HOST, 
+ACL_MEMCPY_HOST_TO_DEVICE, 
+ACL_MEMCPY_DEVICE_TO_HOST,
+ACL_MEMCPY_DEVICE_TO_DEVICE, 
+} aclrtMemcpyKind;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>aclrtMemcpyKind.ACL_MEMCPY_HOST_TO_HOST</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>aclrtMemcpyKind.ACL_MEMCPY_DEVICE_TO_HOST</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>aclrtMemcpyKind.ACL_MEMCPY_DEVICE_TO_DEVICE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>aclrtMemcpyKind.ACL_MEMCPY_HOST_TO_DEVICE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>cudaMemcpyKind.cudaMemcpyHostToDevice</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>cudaMemcpyKind.cudaMemcpyDeviceToHost</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>cudaMemcpyKind.cudaMemcpyDeviceToDevice</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>cudaMemcpyKind.cudaMemcpyHostToHost</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Host内的内存复制</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Host到Device的内存复制</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Device到Host的内存复制</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Device内或Device间的内存复制</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1402,7 +1516,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1439,19 +1553,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1464,30 +1565,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1497,7 +1574,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1555,35 +1632,11 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1866,80 +1919,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="33.90625" customWidth="1"/>
+    <col min="1" max="1" width="50.26953125" customWidth="1"/>
     <col min="2" max="2" width="32.7265625" customWidth="1"/>
     <col min="3" max="3" width="13.26953125" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="51" customWidth="1"/>
     <col min="5" max="5" width="9.6328125" customWidth="1"/>
     <col min="6" max="6" width="10.6328125" customWidth="1"/>
-    <col min="7" max="7" width="24.6328125" customWidth="1"/>
-    <col min="8" max="8" width="32.90625" customWidth="1"/>
+    <col min="7" max="7" width="34.1796875" customWidth="1"/>
+    <col min="8" max="8" width="31.26953125" customWidth="1"/>
     <col min="9" max="9" width="24.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5">
-      <c r="A1" s="23" t="s">
-        <v>275</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26" t="s">
+      <c r="A1" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" s="22"/>
+      <c r="E1" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>280</v>
+      </c>
       <c r="I1" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.5">
-      <c r="A2" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>276</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>278</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="1:9" ht="26.25" customHeight="1">
+    <row r="2" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="42">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>67</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1948,59 +2001,59 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="42">
+    <row r="4" spans="1:9" ht="56">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>279</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="56">
+      <c r="F4" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="70">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="25.5" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="70">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2009,56 +2062,56 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="25.5" customHeight="1">
+    <row r="7" spans="1:9" ht="30.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>162</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="30.75" customHeight="1">
+      <c r="F7" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="26.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>162</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="26.25" customHeight="1">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="28.5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>3</v>
@@ -2070,110 +2123,110 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="28.5" customHeight="1">
+    <row r="10" spans="1:9" ht="22.5" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="22.5" customHeight="1">
+      <c r="F10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="27.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="I11" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="27.75" customHeight="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I12" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="28">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>176</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="21" customHeight="1">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="56">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>3</v>
@@ -2185,93 +2238,103 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="56">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E16" s="1"/>
+      <c r="F15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="42">
+      <c r="A16" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" s="6"/>
       <c r="F16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>181</v>
       </c>
       <c r="I16" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="56">
       <c r="A17" s="6" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>182</v>
+        <v>160</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>184</v>
       </c>
       <c r="I17" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="56">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>187</v>
@@ -2285,61 +2348,63 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="5" t="s">
-        <v>72</v>
+        <v>159</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="G19" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>188</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="I19" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E20" s="6"/>
+    <row r="20" spans="1:9" ht="28">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="F20" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>189</v>
+        <v>72</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="I20" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="28">
+    <row r="21" spans="1:9" ht="62.25" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>87</v>
@@ -2347,89 +2412,77 @@
       <c r="C21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>193</v>
+      <c r="H21" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="I21" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="62.25" customHeight="1">
+    <row r="22" spans="1:9" ht="27.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="D22" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>219</v>
+      <c r="G22" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="I22" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="27.75" customHeight="1">
+    <row r="23" spans="1:9" ht="19.5" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>198</v>
+        <v>88</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="19.5" customHeight="1">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="28">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>3</v>
@@ -2441,56 +2494,66 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="28">
+    <row r="25" spans="1:9" ht="24.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" ht="24.75" customHeight="1">
+      <c r="F25" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="28">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>204</v>
+      <c r="G26" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="I26" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="28">
+    <row r="27" spans="1:9" ht="21.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>3</v>
@@ -2502,153 +2565,153 @@
       <c r="F27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>200</v>
+      <c r="G27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="I27" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="21.75" customHeight="1">
+    <row r="28" spans="1:9" ht="28">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>203</v>
+        <v>134</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>205</v>
+        <v>169</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="I28" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="28">
+    <row r="29" spans="1:9" ht="48.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" ht="41.25" customHeight="1">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G30" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="84">
+      <c r="A31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" ht="28">
+      <c r="A32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="D32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I32" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="48.75" customHeight="1">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" ht="41.25" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I31" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="84">
-      <c r="A32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" ht="28">
+    <row r="33" spans="1:9" ht="42">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>214</v>
+        <v>160</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>212</v>
+        <v>171</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="I33" s="1">
         <v>0.1</v>
@@ -2656,108 +2719,98 @@
     </row>
     <row r="34" spans="1:9" ht="42">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>160</v>
+        <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="4" t="s">
         <v>172</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I34" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="28">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="I35" s="1">
-        <v>0.2</v>
-      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="28">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" ht="28">
+      <c r="F36" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="84">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="I37" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="84">
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" ht="28">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>3</v>
@@ -2769,56 +2822,56 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="28">
+    <row r="39" spans="1:9" ht="98">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" ht="70">
+      <c r="F39" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="42">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>222</v>
-      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I40" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="42">
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" ht="28">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>3</v>
@@ -2830,12 +2883,12 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="28">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>3</v>
@@ -2847,12 +2900,12 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" ht="56">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>3</v>
@@ -2866,10 +2919,10 @@
     </row>
     <row r="44" spans="1:9" ht="56">
       <c r="A44" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>3</v>
@@ -2883,10 +2936,10 @@
     </row>
     <row r="45" spans="1:9" ht="56">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>3</v>
@@ -2900,10 +2953,10 @@
     </row>
     <row r="46" spans="1:9" ht="56">
       <c r="A46" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>3</v>
@@ -2917,10 +2970,10 @@
     </row>
     <row r="47" spans="1:9" ht="56">
       <c r="A47" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>3</v>
@@ -2932,12 +2985,12 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="56">
+    <row r="48" spans="1:9" ht="28">
       <c r="A48" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>3</v>
@@ -2949,56 +3002,56 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="28">
+    <row r="49" spans="1:9" ht="56">
       <c r="A49" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
+      <c r="F49" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="50" spans="1:9" ht="56">
       <c r="A50" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>226</v>
-      </c>
+      <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I50" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="56">
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" ht="28">
       <c r="A51" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>3</v>
@@ -3010,12 +3063,12 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="28">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>3</v>
@@ -3029,124 +3082,134 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="F53" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="98">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>229</v>
+        <v>72</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="I54" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="98">
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G55" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H55" s="2" t="s">
-        <v>228</v>
+      <c r="H55" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="I55" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" ht="84">
       <c r="A56" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>230</v>
+        <v>160</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="I56" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="84">
       <c r="A57" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="4" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="I57" s="1">
         <v>0.2</v>
@@ -3154,134 +3217,134 @@
     </row>
     <row r="58" spans="1:9" ht="84">
       <c r="A58" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="4" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>237</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I58" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="84">
+    <row r="59" spans="1:9" ht="98">
       <c r="A59" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="4" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="I59" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="98">
+    <row r="60" spans="1:9" ht="84">
       <c r="A60" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="4" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>241</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I60" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="84">
+    <row r="61" spans="1:9" ht="42">
       <c r="A61" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>151</v>
+        <v>248</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="4" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="I61" s="1">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="42">
       <c r="A62" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>249</v>
+        <v>145</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="4" t="s">
-        <v>174</v>
+        <v>72</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="I62" s="1">
         <v>0.1</v>
@@ -3289,107 +3352,107 @@
     </row>
     <row r="63" spans="1:9" ht="42">
       <c r="A63" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G63" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="H63" s="2" t="s">
+      <c r="G63" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>254</v>
       </c>
       <c r="I63" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="42">
+    <row r="64" spans="1:9" ht="112">
       <c r="A64" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>255</v>
+        <v>160</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="I64" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="112">
+    <row r="65" spans="1:9" ht="126">
       <c r="A65" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="4" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="I65" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="126">
+    <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>130</v>
+        <v>156</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>288</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>148</v>
+        <v>256</v>
       </c>
       <c r="E66" s="1"/>
-      <c r="F66" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>247</v>
+      <c r="F66" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="I66" s="1">
         <v>0.1</v>
@@ -3397,74 +3460,80 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B67" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="C67" s="4" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="12" t="s">
-        <v>259</v>
+        <v>160</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="I67" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="68" spans="1:9">
-      <c r="A68" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B68" s="1"/>
+      <c r="A68" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>286</v>
+      </c>
       <c r="C68" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E68" s="1"/>
-      <c r="F68" s="12" t="s">
-        <v>160</v>
+      <c r="D68" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E68" s="6"/>
+      <c r="F68" s="4" t="s">
+        <v>173</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>267</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="I68" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B69" s="6"/>
+      <c r="A69" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="C69" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="E69" s="6"/>
+        <v>160</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E69" s="1"/>
       <c r="F69" s="4" t="s">
-        <v>174</v>
+        <v>3</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>268</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I69" s="1">
         <v>0.1</v>
@@ -3472,176 +3541,307 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="4" t="s">
-        <v>160</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C70" s="4"/>
       <c r="D70" s="1" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="E70" s="1"/>
-      <c r="F70" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>264</v>
-      </c>
+      <c r="F70" s="4"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
       <c r="I70" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="84">
+    <row r="71" spans="1:9" ht="98">
       <c r="A71" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="C71" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>270</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="4" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I71" s="1">
         <v>0.2</v>
       </c>
     </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="84">
+      <c r="A74" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="E74" s="1"/>
+      <c r="F74" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="函数说明" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="C32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="C41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="C42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="C44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="C51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="C52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="C53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="C55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="C56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="C57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="C58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="C59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="C60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="C61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="C62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="C64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="C65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="C66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="C68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="C67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="C70" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C2" r:id="rId1" display="函数说明" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="C67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="C66" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
     <hyperlink ref="C71" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="C69" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="F8" r:id="rId70" location="group__CUDART__ERROR_1g3529f94cb530a83a76613616782bd233" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="F11" r:id="rId71" location="group__CUDART__DEVICE_1g159587909ffa0791bbe4b40187a4c6bb" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="F12" r:id="rId72" location="group__CUDART__DEVICE_1gef69dd5c6d0206c2b8d099abac61f217" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="F13" r:id="rId73" location="group__CUDART__DEVICE_1g80861db2ce7c29b6e8055af8ae01bc78" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="F16" r:id="rId74" location="group__CUDART__DEVICE_1g18808e54893cfcaafefeab31a73cc55f" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="F17" r:id="rId75" location="group__CUDA__CTX_1g65dc0012348bc84810e2103a40d8e2cf" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="F18" r:id="rId76" location="group__CUDA__CTX_1g27a365aebb0eb548166309f58a1e8b8e" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="F20" r:id="rId77" location="group__CUDA__CTX_1g8f13165846b73750693640fb3e8380d0" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="F19" r:id="rId78" location="group__CUDA__CTX_1gbe562ee6258b4fcc272ca6478ca2a2f7" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="F21" r:id="rId79" location="group__CUDART__STREAM_1g6a3c4b819e6a994c26d0c4824a4c80da" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="F22" r:id="rId80" location="group__CUDART__STREAM_1ge2be9e9858849bf62ba4a8b66d1c3540" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="F26" r:id="rId81" location="group__CUDART__EVENT_1g7c581e3613a2110ba4d4e7fd5c7da418" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="F27" r:id="rId82" location="group__CUDART__EVENT_1g7b317e07ff385d85aa656204b971a042" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="F28" r:id="rId83" location="group__CUDART__EVENT_1g2cb6baa0830a1cd0bd957bfd8705045b" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="F29" r:id="rId84" location="group__CUDART__EVENT_1gf4fcb74343aa689f4159791967868446" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="F31" r:id="rId85" location="group__CUDART__EVENT_1g2bf738909b4a059023537eaa29d8a5b7" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="F23" r:id="rId86" location="group__CUDART__STREAM_1gfda584f1788ca983cb21c5f4d2033a62" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="F33" r:id="rId87" location="group__CUDART__EVENT_1g949aa42b30ae9e622f6ba0787129ff22" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="F34" r:id="rId88" location="group__CUDART__EVENT_1g40159125411db92c835edb46a0989cd6" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="F35" r:id="rId89" location="group__CUDART__STREAM_1gc301fd024e6fd4a17074d229d4504077" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="F37" r:id="rId90" location="group__CUDART__STREAM_1g82b5784f674c17c6df64affe618bf45e" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="F40" r:id="rId91" location="group__CUDART__STREAM_1g74aa9f4b1c2f12d994bf13876a5a2498" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="F50" r:id="rId92" location="group__CUDART__MEMORY_1g37d37965bfb4803b6d4e59ff26856356" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="F54" r:id="rId93" location="group__CUDART__MEMORY_1ga042655cbbf3408f01061652a075e094" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="F55" r:id="rId94" location="group__CUDART__MEMORY_1gab84100ae1fa1b12eaca660207ef585b" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="F56" r:id="rId95" location="group__CUDART__MEMORY_1g71c078689c17627566b2a91989184969" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="F57" r:id="rId96" location="group__CUDART__MEMORY_1gf7338650f7683c51ee26aadc6973c63a" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="F58" r:id="rId97" location="group__CUDART__MEMORY_1g7c9761e21d9f0999fd136c51e7b9b2a0" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="F59" r:id="rId98" location="group__CUDART__MEMORY_1gc263dbe6574220cc776b45438fc351e8" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="F60" r:id="rId99" location="group__CUDART__MEMORY_1g85073372f776b4c4d5f89f7124b7bf79" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="F61" r:id="rId100" location="group__CUDART__MEMORY_1g376b97f5ab20321ca46f7cfa9511b978" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="F65" r:id="rId101" location="group__CUDART__MEMORY_1g3a58270f6775efe56c65ac47843e7cee" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="F66" r:id="rId102" location="group__CUDART__MEMORY_1ge529b926e8fb574c2666a9a1d58b0dc1" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="F62" r:id="rId103" location="group__CUDART__PEER_1g4db0d04e44995d5c1c34be4ecc863f22" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="F63" r:id="rId104" location="group__CUDART__PEER_1g2b0adabf90db37e5cfddc92cbb2589f3" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="F64" r:id="rId105" location="group__CUDART__PEER_1g9663734ad02653207ad6836053bf572e" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="F67" r:id="rId106" location="group__CUDART__TYPES_1ge15d9c8b7a240312b533d6122558085a" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="F68" r:id="rId107" location="group__CUDART__TYPES_1gea2f543a9fc0e52fe4ae712920fd1247" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="F69" r:id="rId108" location="group__CUDA__TYPES_1gf9f5bd81658f866613785b3a0bb7d7d9" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="F70" r:id="rId109" location="group__CUDART__TYPES_1gf599e5b8b829ce7db0f5216928f6ecb6" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="C68" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="F7" r:id="rId70" location="group__CUDART__ERROR_1g3529f94cb530a83a76613616782bd233" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="F10" r:id="rId71" location="group__CUDART__DEVICE_1g159587909ffa0791bbe4b40187a4c6bb" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="F11" r:id="rId72" location="group__CUDART__DEVICE_1gef69dd5c6d0206c2b8d099abac61f217" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="F12" r:id="rId73" location="group__CUDART__DEVICE_1g80861db2ce7c29b6e8055af8ae01bc78" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="F15" r:id="rId74" location="group__CUDART__DEVICE_1g18808e54893cfcaafefeab31a73cc55f" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="F16" r:id="rId75" location="group__CUDA__CTX_1g65dc0012348bc84810e2103a40d8e2cf" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="F17" r:id="rId76" location="group__CUDA__CTX_1g27a365aebb0eb548166309f58a1e8b8e" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="F19" r:id="rId77" location="group__CUDA__CTX_1g8f13165846b73750693640fb3e8380d0" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="F18" r:id="rId78" location="group__CUDA__CTX_1gbe562ee6258b4fcc272ca6478ca2a2f7" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="F20" r:id="rId79" location="group__CUDART__STREAM_1g6a3c4b819e6a994c26d0c4824a4c80da" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="F21" r:id="rId80" location="group__CUDART__STREAM_1ge2be9e9858849bf62ba4a8b66d1c3540" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="F25" r:id="rId81" location="group__CUDART__EVENT_1g7c581e3613a2110ba4d4e7fd5c7da418" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="F26" r:id="rId82" location="group__CUDART__EVENT_1g7b317e07ff385d85aa656204b971a042" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="F27" r:id="rId83" location="group__CUDART__EVENT_1g2cb6baa0830a1cd0bd957bfd8705045b" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="F28" r:id="rId84" location="group__CUDART__EVENT_1gf4fcb74343aa689f4159791967868446" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="F30" r:id="rId85" location="group__CUDART__EVENT_1g2bf738909b4a059023537eaa29d8a5b7" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="F22" r:id="rId86" location="group__CUDART__STREAM_1gfda584f1788ca983cb21c5f4d2033a62" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="F32" r:id="rId87" location="group__CUDART__EVENT_1g949aa42b30ae9e622f6ba0787129ff22" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="F33" r:id="rId88" location="group__CUDART__EVENT_1g40159125411db92c835edb46a0989cd6" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="F34" r:id="rId89" location="group__CUDART__STREAM_1gc301fd024e6fd4a17074d229d4504077" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="F36" r:id="rId90" location="group__CUDART__STREAM_1g82b5784f674c17c6df64affe618bf45e" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="F39" r:id="rId91" location="group__CUDART__STREAM_1g74aa9f4b1c2f12d994bf13876a5a2498" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="F49" r:id="rId92" location="group__CUDART__MEMORY_1g37d37965bfb4803b6d4e59ff26856356" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="F53" r:id="rId93" location="group__CUDART__MEMORY_1ga042655cbbf3408f01061652a075e094" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="F54" r:id="rId94" location="group__CUDART__MEMORY_1gab84100ae1fa1b12eaca660207ef585b" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="F55" r:id="rId95" location="group__CUDART__MEMORY_1g71c078689c17627566b2a91989184969" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="F56" r:id="rId96" location="group__CUDART__MEMORY_1gf7338650f7683c51ee26aadc6973c63a" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="F57" r:id="rId97" location="group__CUDART__MEMORY_1g7c9761e21d9f0999fd136c51e7b9b2a0" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="F58" r:id="rId98" location="group__CUDART__MEMORY_1gc263dbe6574220cc776b45438fc351e8" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="F59" r:id="rId99" location="group__CUDART__MEMORY_1g85073372f776b4c4d5f89f7124b7bf79" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="F60" r:id="rId100" location="group__CUDART__MEMORY_1g376b97f5ab20321ca46f7cfa9511b978" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="F64" r:id="rId101" location="group__CUDART__MEMORY_1g3a58270f6775efe56c65ac47843e7cee" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="F65" r:id="rId102" location="group__CUDART__MEMORY_1ge529b926e8fb574c2666a9a1d58b0dc1" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="F61" r:id="rId103" location="group__CUDART__PEER_1g4db0d04e44995d5c1c34be4ecc863f22" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="F62" r:id="rId104" location="group__CUDART__PEER_1g2b0adabf90db37e5cfddc92cbb2589f3" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="F63" r:id="rId105" location="group__CUDART__PEER_1g9663734ad02653207ad6836053bf572e" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="F66" r:id="rId106" location="group__CUDART__TYPES_1ge15d9c8b7a240312b533d6122558085a" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="F67" r:id="rId107" location="group__CUDART__TYPES_1gea2f543a9fc0e52fe4ae712920fd1247" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="F68" r:id="rId108" location="group__CUDA__TYPES_1gf9f5bd81658f866613785b3a0bb7d7d9" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="F69" r:id="rId109" location="group__CUDART__TYPES_1gf599e5b8b829ce7db0f5216928f6ecb6" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
     <hyperlink ref="F71" r:id="rId110" location="group__CUDART__TYPES_1g13de56a8fe75569530ecc3a3106e9b6d" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="F5" r:id="rId111" location="group__CUDART____VERSION_1g0e3952c7802fd730432180f1f4a6cdc6" xr:uid="{3A01CD8A-CF33-4683-8954-91BAF1C06320}"/>
+    <hyperlink ref="F4" r:id="rId111" location="group__CUDART____VERSION_1g0e3952c7802fd730432180f1f4a6cdc6" xr:uid="{3A01CD8A-CF33-4683-8954-91BAF1C06320}"/>
+    <hyperlink ref="C74" r:id="rId112" xr:uid="{14D87FEF-EB62-41AE-AE36-67A3BA0BA3F4}"/>
+    <hyperlink ref="F74" r:id="rId113" location="group__CUDART__TYPES_1g18fa99055ee694244a270e4d5101e95b" xr:uid="{686CDA3C-47A8-4405-8C32-87DA565F7D09}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId112"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId114"/>
 </worksheet>
 </file>
</xml_diff>